<commit_message>
Update feature open new tab commit
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/DataImport.xlsx
+++ b/src/test/resources/Data/DataImport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phuonganh.tran\Documents\Tester\Git\LearnNewFeatures-Meclip\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7916902-F50D-479E-81E8-81F9D23B0467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86027F10-8FD9-478B-B182-840A35BF9E9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>phone</t>
   </si>
@@ -47,26 +47,53 @@
     <t>v26m20</t>
   </si>
   <si>
-    <t>http://meclip.vn/watch?v=669e2cc680bfb76ebabac386</t>
-  </si>
-  <si>
-    <t>http://meclip.vn/watch?v=6014047580bfb73c12e823b4</t>
-  </si>
-  <si>
-    <t>http://meclip.vn/watch?v=6749882280bfb761a24af6b3</t>
-  </si>
-  <si>
-    <t>http://meclip.vn/watch?v=61b2cbf480bfb7459f5cb7ee</t>
-  </si>
-  <si>
-    <t>http://meclip.vn/watch?v=611b3cdc80bfb7594cbef39c</t>
+    <t>http://meclip.vn/watch?v=626f7c8980bfb762b95c2002</t>
+  </si>
+  <si>
+    <t>http://meclip.vn/watch?v=626f7a5980bfb762b95c1f80</t>
+  </si>
+  <si>
+    <t>http://meclip.vn/watch?v=626f7b7680bfb762b95c1fc1</t>
+  </si>
+  <si>
+    <t>http://meclip.vn/watch?v=626f7c4180bfb762b95c1ff2</t>
+  </si>
+  <si>
+    <t>http://meclip.vn/watch?v=626f7b9d80bfb762b95c1fc8</t>
+  </si>
+  <si>
+    <t>http://meclip.vn/watch?v=626f7cad80bfb762b95c200c</t>
+  </si>
+  <si>
+    <t>http://meclip.vn/watch?v=626f797680bfb762b95c1f63</t>
+  </si>
+  <si>
+    <t>http://meclip.vn/watch?v=626f7a3780bfb762b95c1f7c</t>
+  </si>
+  <si>
+    <t>http://meclip.vn/watch?v=626f7c1c80bfb762b95c1fec</t>
+  </si>
+  <si>
+    <t>http://meclip.vn/watch?v=626f7b2a80bfb762b95c1fb3</t>
+  </si>
+  <si>
+    <t>http://meclip.vn/watch?v=626f79b180bfb762b95c1f6a</t>
+  </si>
+  <si>
+    <t>http://meclip.vn/watch?v=626f78f580bfb762b95c1f46</t>
+  </si>
+  <si>
+    <t>http://meclip.vn/watch?v=626f619180bfb762b95c1bb0</t>
+  </si>
+  <si>
+    <t>http://meclip.vn/watch?v=626d292d80bfb762b95b93cf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -76,13 +103,6 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -109,18 +129,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -370,7 +387,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -380,10 +397,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -394,44 +411,82 @@
       </c>
     </row>
     <row r="2" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" t="s">
         <v>12</v>
       </c>
     </row>
+    <row r="8" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" xr:uid="{118080F8-0676-4CCC-B81D-D06EDD5A18B3}"/>
-    <hyperlink ref="A4" r:id="rId2" xr:uid="{A96691AB-999F-46B0-93FD-C4638EB43EBD}"/>
-    <hyperlink ref="A5" r:id="rId3" xr:uid="{C31250C6-7A42-4E03-87A1-3E98A7990BA1}"/>
-    <hyperlink ref="A6" r:id="rId4" xr:uid="{B2CF2384-AEEB-45F2-9341-CA244CBBC6E1}"/>
-    <hyperlink ref="A7" r:id="rId5" xr:uid="{047008E9-BB08-4183-81C5-16B9A4A199C3}"/>
-  </hyperlinks>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>